<commit_message>
C4.5 with REP. Real Data & Sample Data
</commit_message>
<xml_diff>
--- a/Data/ManualBeasiswaBI.xlsx
+++ b/Data/ManualBeasiswaBI.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\RekomendasiBeasiswa\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36D5510-978B-49B1-B3AC-87E2C70D8EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12469ECF-503D-44C5-A03C-09AE1CF20648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{BE3E6305-258F-4057-BF6A-3D3AEE71B70E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{BE3E6305-258F-4057-BF6A-3D3AEE71B70E}"/>
   </bookViews>
   <sheets>
     <sheet name="Train" sheetId="1" r:id="rId1"/>
-    <sheet name="Test" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Binning_Iter1" sheetId="4" r:id="rId2"/>
+    <sheet name="Test" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="186">
   <si>
     <t>Status Beasiswa BI</t>
   </si>
@@ -549,6 +550,42 @@
   </si>
   <si>
     <t>Tanggungan Ortu</t>
+  </si>
+  <si>
+    <t>Perhitungan Entrophy</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Jumlah Kasus</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Log 2</t>
+  </si>
+  <si>
+    <t>Jmlh Kasus/Total</t>
+  </si>
+  <si>
+    <t>Entropy ( E ) =</t>
+  </si>
+  <si>
+    <t>Pemecahan Fitur NR 1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Gain</t>
   </si>
 </sst>
 </file>
@@ -650,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -669,6 +706,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -984,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70217A22-942D-4EE5-9513-7BF2E6F9E317}">
-  <dimension ref="A1:N239"/>
+  <dimension ref="A1:T239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C237" sqref="C2:C237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,11 +1039,14 @@
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>161</v>
@@ -1032,7 +1079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1069,10 +1116,17 @@
       <c r="L2" s="4">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O2">
+        <f>-(((COUNTIF($B$2:$B$237,"Iya")/COUNTA($B$2:$B$237))*(IMLOG2(COUNTIF($B$2:$B$237,"Iya")/COUNTA($B$2:$B$237))))+((COUNTIF($B$2:$B$237,"Tidak")/COUNTA($B$2:$B$237))*(IMLOG2(COUNTIF($B$2:$B$237,"Tidak")/COUNTA($B$2:$B$237)))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>1+A2</f>
+        <f t="shared" ref="A3:A37" si="0">1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1108,10 +1162,16 @@
       <c r="L3" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>1+A3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1147,10 +1207,22 @@
       <c r="L4" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>1+A4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1186,10 +1258,25 @@
       <c r="L5" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="3">
+        <f>COUNTIF($B$2:$B$237,"Iya")</f>
+        <v>118</v>
+      </c>
+      <c r="P5" s="9">
+        <f>O5/$O$7</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="8" t="str">
+        <f>IMLOG2(P5)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>1+A5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1225,10 +1312,25 @@
       <c r="L6" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="O6" s="3">
+        <f>COUNTIF($B$2:$B$237,"Tidak")</f>
+        <v>118</v>
+      </c>
+      <c r="P6" s="9">
+        <f>O6/$O$7</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="8" t="str">
+        <f>IMLOG2(P6)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>1+A6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1264,10 +1366,19 @@
       <c r="L7" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="O7" s="9">
+        <f>COUNTA($B$2:$B$237)</f>
+        <v>236</v>
+      </c>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>1+A7</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1304,9 +1415,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>1+A8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1342,10 +1453,13 @@
       <c r="L9" s="3">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>1+A9</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1381,10 +1495,28 @@
       <c r="L10" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>167</v>
+      </c>
+      <c r="P10" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>182</v>
+      </c>
+      <c r="R10" t="s">
+        <v>183</v>
+      </c>
+      <c r="S10" t="s">
+        <v>184</v>
+      </c>
+      <c r="T10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>1+A10</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1421,9 +1553,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>1+A11</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1460,9 +1592,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>1+A12</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1499,9 +1631,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>1+A13</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1538,9 +1670,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>1+A14</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1577,9 +1709,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>1+A15</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1657,7 +1789,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>1+A17</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1696,7 +1828,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>1+A18</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1735,7 +1867,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>1+A19</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1774,7 +1906,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>1+A20</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1813,7 +1945,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>1+A21</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1852,7 +1984,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>1+A22</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1891,7 +2023,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>1+A23</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1930,7 +2062,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>1+A24</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1969,7 +2101,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>1+A25</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2008,7 +2140,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>1+A26</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2047,7 +2179,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>1+A27</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2086,7 +2218,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>1+A28</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2125,7 +2257,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>1+A29</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2164,7 +2296,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>1+A30</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2203,7 +2335,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>1+A31</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2242,7 +2374,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>1+A32</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2281,7 +2413,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>1+A33</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2320,7 +2452,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>1+A34</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2359,7 +2491,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>1+A35</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2398,7 +2530,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>1+A36</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2437,7 +2569,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" ref="A38:A101" si="0">1+A37</f>
+        <f t="shared" ref="A38:A101" si="1">1+A37</f>
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2476,7 +2608,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2515,7 +2647,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2554,7 +2686,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2593,7 +2725,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2632,7 +2764,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2671,7 +2803,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2710,7 +2842,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2749,7 +2881,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2788,7 +2920,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2827,7 +2959,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2866,7 +2998,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2905,7 +3037,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2944,7 +3076,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2983,7 +3115,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -3022,7 +3154,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -3061,7 +3193,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3100,7 +3232,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -3139,7 +3271,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3178,7 +3310,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3217,7 +3349,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3256,7 +3388,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -3295,7 +3427,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -3334,7 +3466,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -3373,7 +3505,7 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -3412,7 +3544,7 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3451,7 +3583,7 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -3490,7 +3622,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -3529,7 +3661,7 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -3568,7 +3700,7 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -3607,7 +3739,7 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -3646,7 +3778,7 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -3685,7 +3817,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -3724,7 +3856,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -3763,7 +3895,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -3802,7 +3934,7 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -3841,7 +3973,7 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -3880,7 +4012,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -3919,7 +4051,7 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -3958,7 +4090,7 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -3997,7 +4129,7 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -4036,7 +4168,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -4075,7 +4207,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -4114,7 +4246,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -4153,7 +4285,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -4192,7 +4324,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -4231,7 +4363,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -4270,7 +4402,7 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -4309,7 +4441,7 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -4348,7 +4480,7 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -4387,7 +4519,7 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -4426,7 +4558,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -4465,7 +4597,7 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -4504,7 +4636,7 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -4543,7 +4675,7 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -4582,7 +4714,7 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -4621,7 +4753,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -4660,7 +4792,7 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -4699,7 +4831,7 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -4738,7 +4870,7 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -4777,7 +4909,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -4816,7 +4948,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -4855,7 +4987,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -4894,7 +5026,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -4933,7 +5065,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" ref="A102:A165" si="1">1+A101</f>
+        <f t="shared" ref="A102:A165" si="2">1+A101</f>
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -4972,7 +5104,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -5011,7 +5143,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -5050,7 +5182,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -5089,7 +5221,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -5128,7 +5260,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -5167,7 +5299,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -5206,7 +5338,7 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -5245,7 +5377,7 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -5284,7 +5416,7 @@
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -5323,7 +5455,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -5362,7 +5494,7 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -5401,7 +5533,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -5440,7 +5572,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -5479,7 +5611,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
@@ -5518,7 +5650,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -5557,7 +5689,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -5596,7 +5728,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -5635,7 +5767,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -5674,7 +5806,7 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -5713,7 +5845,7 @@
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -5752,7 +5884,7 @@
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -5791,7 +5923,7 @@
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -5830,7 +5962,7 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -5869,7 +6001,7 @@
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -5908,7 +6040,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -5947,7 +6079,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -5986,7 +6118,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
@@ -6025,7 +6157,7 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -6064,7 +6196,7 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -6103,7 +6235,7 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -6142,7 +6274,7 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
@@ -6181,7 +6313,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -6220,7 +6352,7 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -6259,7 +6391,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
@@ -6298,7 +6430,7 @@
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -6337,7 +6469,7 @@
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -6376,7 +6508,7 @@
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -6415,7 +6547,7 @@
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -6454,7 +6586,7 @@
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
@@ -6493,7 +6625,7 @@
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -6532,7 +6664,7 @@
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
@@ -6571,7 +6703,7 @@
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -6610,7 +6742,7 @@
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -6649,7 +6781,7 @@
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -6688,7 +6820,7 @@
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -6727,7 +6859,7 @@
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -6766,7 +6898,7 @@
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -6805,7 +6937,7 @@
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -6844,7 +6976,7 @@
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
@@ -6883,7 +7015,7 @@
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
@@ -6922,7 +7054,7 @@
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -6961,7 +7093,7 @@
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
@@ -7000,7 +7132,7 @@
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
@@ -7039,7 +7171,7 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
@@ -7078,7 +7210,7 @@
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -7117,7 +7249,7 @@
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -7156,7 +7288,7 @@
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
@@ -7195,7 +7327,7 @@
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -7234,7 +7366,7 @@
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
@@ -7273,7 +7405,7 @@
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
@@ -7312,7 +7444,7 @@
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
@@ -7351,7 +7483,7 @@
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
@@ -7390,7 +7522,7 @@
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
@@ -7429,7 +7561,7 @@
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166">
-        <f t="shared" ref="A166:A229" si="2">1+A165</f>
+        <f t="shared" ref="A166:A229" si="3">1+A165</f>
         <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
@@ -7468,7 +7600,7 @@
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
@@ -7507,7 +7639,7 @@
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -7546,7 +7678,7 @@
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
@@ -7585,7 +7717,7 @@
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -7624,7 +7756,7 @@
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
@@ -7663,7 +7795,7 @@
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
@@ -7702,7 +7834,7 @@
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
@@ -7741,7 +7873,7 @@
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
@@ -7780,7 +7912,7 @@
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -7819,7 +7951,7 @@
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
@@ -7858,7 +7990,7 @@
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
@@ -7897,7 +8029,7 @@
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
@@ -7936,7 +8068,7 @@
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="B179" s="3" t="s">
@@ -7975,7 +8107,7 @@
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>179</v>
       </c>
       <c r="B180" s="3" t="s">
@@ -8014,7 +8146,7 @@
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="B181" s="3" t="s">
@@ -8053,7 +8185,7 @@
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>181</v>
       </c>
       <c r="B182" s="3" t="s">
@@ -8092,7 +8224,7 @@
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>182</v>
       </c>
       <c r="B183" s="3" t="s">
@@ -8131,7 +8263,7 @@
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>183</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -8170,7 +8302,7 @@
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>184</v>
       </c>
       <c r="B185" s="3" t="s">
@@ -8209,7 +8341,7 @@
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>185</v>
       </c>
       <c r="B186" s="3" t="s">
@@ -8248,7 +8380,7 @@
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>186</v>
       </c>
       <c r="B187" s="3" t="s">
@@ -8287,7 +8419,7 @@
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>187</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -8326,7 +8458,7 @@
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>188</v>
       </c>
       <c r="B189" s="3" t="s">
@@ -8365,7 +8497,7 @@
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189</v>
       </c>
       <c r="B190" s="3" t="s">
@@ -8404,7 +8536,7 @@
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
       <c r="B191" s="3" t="s">
@@ -8443,7 +8575,7 @@
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>191</v>
       </c>
       <c r="B192" s="3" t="s">
@@ -8482,7 +8614,7 @@
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>192</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -8521,7 +8653,7 @@
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>193</v>
       </c>
       <c r="B194" s="3" t="s">
@@ -8560,7 +8692,7 @@
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>194</v>
       </c>
       <c r="B195" s="3" t="s">
@@ -8599,7 +8731,7 @@
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>195</v>
       </c>
       <c r="B196" s="3" t="s">
@@ -8638,7 +8770,7 @@
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>196</v>
       </c>
       <c r="B197" s="3" t="s">
@@ -8677,7 +8809,7 @@
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="B198" s="3" t="s">
@@ -8716,7 +8848,7 @@
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>198</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -8755,7 +8887,7 @@
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>199</v>
       </c>
       <c r="B200" s="3" t="s">
@@ -8794,7 +8926,7 @@
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
       <c r="B201" s="3" t="s">
@@ -8833,7 +8965,7 @@
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>201</v>
       </c>
       <c r="B202" s="3" t="s">
@@ -8872,7 +9004,7 @@
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>202</v>
       </c>
       <c r="B203" s="3" t="s">
@@ -8911,7 +9043,7 @@
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>203</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -8950,7 +9082,7 @@
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>204</v>
       </c>
       <c r="B205" s="3" t="s">
@@ -8989,7 +9121,7 @@
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>205</v>
       </c>
       <c r="B206" s="3" t="s">
@@ -9028,7 +9160,7 @@
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>206</v>
       </c>
       <c r="B207" s="3" t="s">
@@ -9067,7 +9199,7 @@
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>207</v>
       </c>
       <c r="B208" s="3" t="s">
@@ -9106,7 +9238,7 @@
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>208</v>
       </c>
       <c r="B209" s="3" t="s">
@@ -9145,7 +9277,7 @@
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>209</v>
       </c>
       <c r="B210" s="3" t="s">
@@ -9184,7 +9316,7 @@
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>210</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -9223,7 +9355,7 @@
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>211</v>
       </c>
       <c r="B212" s="3" t="s">
@@ -9262,7 +9394,7 @@
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>212</v>
       </c>
       <c r="B213" s="3" t="s">
@@ -9301,7 +9433,7 @@
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>213</v>
       </c>
       <c r="B214" s="3" t="s">
@@ -9340,7 +9472,7 @@
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>214</v>
       </c>
       <c r="B215" s="3" t="s">
@@ -9379,7 +9511,7 @@
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>215</v>
       </c>
       <c r="B216" s="3" t="s">
@@ -9418,7 +9550,7 @@
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>216</v>
       </c>
       <c r="B217" s="3" t="s">
@@ -9457,7 +9589,7 @@
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -9496,7 +9628,7 @@
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>218</v>
       </c>
       <c r="B219" s="3" t="s">
@@ -9535,7 +9667,7 @@
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>219</v>
       </c>
       <c r="B220" s="3" t="s">
@@ -9574,7 +9706,7 @@
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="B221" s="3" t="s">
@@ -9613,7 +9745,7 @@
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>221</v>
       </c>
       <c r="B222" s="3" t="s">
@@ -9652,7 +9784,7 @@
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>222</v>
       </c>
       <c r="B223" s="3" t="s">
@@ -9691,7 +9823,7 @@
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>223</v>
       </c>
       <c r="B224" s="3" t="s">
@@ -9730,7 +9862,7 @@
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>224</v>
       </c>
       <c r="B225" s="3" t="s">
@@ -9769,7 +9901,7 @@
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="B226" s="3" t="s">
@@ -9808,7 +9940,7 @@
     </row>
     <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>226</v>
       </c>
       <c r="B227" s="3" t="s">
@@ -9847,7 +9979,7 @@
     </row>
     <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>227</v>
       </c>
       <c r="B228" s="3" t="s">
@@ -9886,7 +10018,7 @@
     </row>
     <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>228</v>
       </c>
       <c r="B229" s="3" t="s">
@@ -9925,7 +10057,7 @@
     </row>
     <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230">
-        <f t="shared" ref="A230:A237" si="3">1+A229</f>
+        <f t="shared" ref="A230:A237" si="4">1+A229</f>
         <v>229</v>
       </c>
       <c r="B230" s="3" t="s">
@@ -9964,7 +10096,7 @@
     </row>
     <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>230</v>
       </c>
       <c r="B231" s="3" t="s">
@@ -10003,7 +10135,7 @@
     </row>
     <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>231</v>
       </c>
       <c r="B232" s="3" t="s">
@@ -10042,7 +10174,7 @@
     </row>
     <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>232</v>
       </c>
       <c r="B233" s="3" t="s">
@@ -10081,7 +10213,7 @@
     </row>
     <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>233</v>
       </c>
       <c r="B234" s="3" t="s">
@@ -10120,7 +10252,7 @@
     </row>
     <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>234</v>
       </c>
       <c r="B235" s="3" t="s">
@@ -10159,7 +10291,7 @@
     </row>
     <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>235</v>
       </c>
       <c r="B236" s="3" t="s">
@@ -10195,10 +10327,14 @@
       <c r="L236" s="3">
         <v>20</v>
       </c>
+      <c r="N236">
+        <f>20%*B239</f>
+        <v>23.6</v>
+      </c>
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>236</v>
       </c>
       <c r="B237" s="3" t="s">
@@ -10233,10 +10369,6 @@
       </c>
       <c r="L237" s="3">
         <v>18</v>
-      </c>
-      <c r="N237">
-        <f>20%*B239</f>
-        <v>23.6</v>
       </c>
     </row>
     <row r="238" spans="1:14" x14ac:dyDescent="0.25">
@@ -10272,12 +10404,1219 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="N3:Q3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8B7E6E-4D43-4B59-BB7A-9F787FDB2DC3}">
+  <dimension ref="A1:A237"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63584820-4893-4B05-80F0-C606EA0B8017}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
@@ -10378,7 +11717,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>1+A2</f>
+        <f t="shared" ref="A3:A31" si="0">1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -10417,7 +11756,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>1+A3</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -10456,7 +11795,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>1+A4</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -10495,7 +11834,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>1+A5</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -10534,7 +11873,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>1+A6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -10573,7 +11912,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>1+A7</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -10612,7 +11951,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>1+A8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -10651,7 +11990,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>1+A9</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -10690,7 +12029,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>1+A10</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -10729,7 +12068,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>1+A11</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -10768,7 +12107,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>1+A12</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -10807,7 +12146,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>1+A13</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -10846,7 +12185,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>1+A14</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -10885,7 +12224,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>1+A15</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -10924,7 +12263,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>1+A16</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -10963,7 +12302,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>1+A17</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -11002,7 +12341,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>1+A18</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -11041,7 +12380,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>1+A19</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -11080,7 +12419,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>1+A20</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -11119,7 +12458,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>1+A21</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -11158,7 +12497,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>1+A22</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -11197,7 +12536,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>1+A23</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -11236,7 +12575,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>1+A24</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -11275,7 +12614,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>1+A25</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -11314,7 +12653,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>1+A26</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -11353,7 +12692,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>1+A27</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -11392,7 +12731,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>1+A28</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -11431,7 +12770,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>1+A29</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -11470,7 +12809,7 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>1+A30</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -11509,7 +12848,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" ref="A32:A61" si="0">1+A31</f>
+        <f t="shared" ref="A32:A61" si="1">1+A31</f>
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -11548,7 +12887,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -11587,7 +12926,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -11626,7 +12965,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -11665,7 +13004,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -11704,7 +13043,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -11743,7 +13082,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -11782,7 +13121,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -11821,7 +13160,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -11860,7 +13199,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -11899,7 +13238,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -11938,7 +13277,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -11977,7 +13316,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -12016,7 +13355,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -12055,7 +13394,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -12094,7 +13433,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -12133,7 +13472,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -12172,7 +13511,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -12211,7 +13550,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -12250,7 +13589,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -12289,7 +13628,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -12328,7 +13667,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -12367,7 +13706,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -12406,7 +13745,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -12445,7 +13784,7 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -12484,7 +13823,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -12523,7 +13862,7 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -12562,7 +13901,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -12601,7 +13940,7 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -12640,7 +13979,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -12682,11 +14021,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C31D95E-E154-4520-B568-9FC712875A85}">
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>